<commit_message>
Spare from BL11I now working
</commit_message>
<xml_diff>
--- a/Focus table.xlsx
+++ b/Focus table.xlsx
@@ -5,81 +5,98 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
-    <t xml:space="preserve">GAP</t>
+    <t>GAP</t>
   </si>
   <si>
-    <t xml:space="preserve">CEN</t>
+    <t>CEN</t>
   </si>
   <si>
-    <t xml:space="preserve">Lens 1</t>
+    <t>Lens 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Lens 2</t>
+    <t>Lens 2</t>
   </si>
   <si>
-    <t xml:space="preserve">Loop height</t>
+    <t>Loop height</t>
   </si>
   <si>
-    <t xml:space="preserve">Mag</t>
+    <t>Mag</t>
   </si>
   <si>
-    <t xml:space="preserve">a</t>
+    <t>a</t>
   </si>
   <si>
-    <t xml:space="preserve">X-h^2</t>
+    <t>X-h^2</t>
   </si>
   <si>
-    <t xml:space="preserve">h</t>
+    <t>h</t>
   </si>
   <si>
-    <t xml:space="preserve">k</t>
+    <t>k</t>
   </si>
   <si>
-    <t xml:space="preserve">X-h</t>
+    <t>X-h</t>
   </si>
   <si>
-    <t xml:space="preserve">a(x-h)^2</t>
+    <t>a(x-h)^2</t>
   </si>
   <si>
-    <t xml:space="preserve">Calculate</t>
+    <t>Calculate</t>
   </si>
   <si>
-    <t xml:space="preserve">Actual</t>
+    <t>Actual</t>
   </si>
   <si>
-    <t xml:space="preserve">poly1</t>
+    <t>poly1</t>
   </si>
   <si>
-    <t xml:space="preserve">poly2</t>
+    <t>poly2</t>
   </si>
   <si>
-    <t xml:space="preserve">poly3</t>
+    <t>poly3</t>
   </si>
   <si>
-    <t xml:space="preserve">poly4</t>
+    <t>poly4</t>
   </si>
   <si>
-    <t xml:space="preserve">poly5</t>
+    <t>poly5</t>
   </si>
   <si>
-    <t xml:space="preserve">poly6</t>
+    <t>poly6</t>
+  </si>
+  <si>
+    <t>BL11I Spare</t>
+  </si>
+  <si>
+    <t>C1=37.5753</t>
+  </si>
+  <si>
+    <t>C2=-0.08591837</t>
+  </si>
+  <si>
+    <t>C3=-0.1905368</t>
+  </si>
+  <si>
+    <t>C4=0.007939368</t>
+  </si>
+  <si>
+    <t>C5=-0.0001079176</t>
+  </si>
+  <si>
+    <t>C6=0.0000004957167</t>
   </si>
 </sst>
 </file>
@@ -87,10 +104,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0.00E+00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -118,6 +135,19 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -162,12 +192,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -246,9 +280,9 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
   <c:chart>
     <c:plotArea>
+      <c:layout/>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -275,15 +309,6 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$6:$B$20</c:f>
@@ -417,15 +442,6 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$B$6:$B$20</c:f>
@@ -559,15 +575,6 @@
               </a:solidFill>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:dLblPos val="r"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$H$29:$H$43</c:f>
@@ -678,17 +685,16 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="29547750"/>
-        <c:axId val="80111649"/>
+        <c:axId val="5801465"/>
+        <c:axId val="69067316"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="29547750"/>
+        <c:axId val="5801465"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -700,30 +706,11 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="80111649"/>
+        <c:crossAx val="69067316"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="80111649"/>
+        <c:axId val="69067316"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -739,7 +726,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -751,27 +737,8 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:uFill>
-                  <a:solidFill>
-                    <a:srgbClr val="ffffff"/>
-                  </a:solidFill>
-                </a:uFill>
-                <a:latin typeface="Calibri"/>
-              </a:defRPr>
-            </a:pPr>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="29547750"/>
+        <c:crossAx val="5801465"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -793,7 +760,6 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -811,15 +777,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>367200</xdr:colOff>
+      <xdr:colOff>394200</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>113760</xdr:rowOff>
+      <xdr:rowOff>104760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>33</xdr:col>
-      <xdr:colOff>258840</xdr:colOff>
+      <xdr:colOff>285480</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>131400</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -827,8 +793,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="10879560" y="1378440"/>
-        <a:ext cx="10287000" cy="5686920"/>
+        <a:off x="10905120" y="1369440"/>
+        <a:ext cx="10287000" cy="5686560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -848,19 +814,19 @@
   </sheetPr>
   <dimension ref="A1:U107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4:B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="7" style="0" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="11" style="0" width="8.67"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.66836734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.66836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.3316326530612"/>
+    <col collapsed="false" hidden="false" max="9" min="7" style="0" width="8.66836734693878"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.9897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.66836734693878"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,7 +1310,7 @@
       </c>
       <c r="N29" s="0" t="n">
         <f aca="false">M29-L29</f>
-        <v>0.181920000000002</v>
+        <v>0.181919999999998</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1379,7 +1345,7 @@
       </c>
       <c r="N30" s="0" t="n">
         <f aca="false">M30-L30</f>
-        <v>0.383520000000004</v>
+        <v>0.383520000000001</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1449,7 +1415,7 @@
       </c>
       <c r="N32" s="0" t="n">
         <f aca="false">M32-L32</f>
-        <v>0.358720000000001</v>
+        <v>0.35872</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1519,7 +1485,7 @@
       </c>
       <c r="N34" s="0" t="n">
         <f aca="false">M34-L34</f>
-        <v>0.129920000000001</v>
+        <v>0.12992</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1659,7 +1625,7 @@
       </c>
       <c r="N38" s="0" t="n">
         <f aca="false">M38-L38</f>
-        <v>0.16032</v>
+        <v>0.160319999999999</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1729,7 +1695,7 @@
       </c>
       <c r="N40" s="0" t="n">
         <f aca="false">M40-L40</f>
-        <v>0.31952</v>
+        <v>0.319519999999999</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1764,7 +1730,7 @@
       </c>
       <c r="N41" s="0" t="n">
         <f aca="false">M41-L41</f>
-        <v>0.18512</v>
+        <v>0.185119999999998</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1834,7 +1800,7 @@
       </c>
       <c r="N43" s="0" t="n">
         <f aca="false">M43-L43</f>
-        <v>-0.561680000000001</v>
+        <v>-0.561680000000004</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2818,11 +2784,227 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E25"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.1122448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="18.7551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>11.5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>20.7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>16.9</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>13.4</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10.2</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>7.5</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>3.65</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>2.65</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>2.25</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="n">
+        <v>3.35</v>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>4.75</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>11.9</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>42</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>4.957167E-007</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>18.5</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>20.3</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>